<commit_message>
update two plots for EH
</commit_message>
<xml_diff>
--- a/analysis/data/stone_artefact_data/GSPhases_BM1.xlsx
+++ b/analysis/data/stone_artefact_data/GSPhases_BM1.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="21195" yWindow="2085" windowWidth="20730" windowHeight="11700" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="21195" yWindow="2085" windowWidth="20730" windowHeight="11700" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="331">
   <si>
     <t>Site</t>
   </si>
@@ -854,13 +855,172 @@
   </si>
   <si>
     <t>Multiple</t>
+  </si>
+  <si>
+    <t>Processed material</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plant </t>
+  </si>
+  <si>
+    <t xml:space="preserve">animal </t>
+  </si>
+  <si>
+    <t xml:space="preserve">pigment </t>
+  </si>
+  <si>
+    <t xml:space="preserve">stone </t>
+  </si>
+  <si>
+    <t xml:space="preserve">metal </t>
+  </si>
+  <si>
+    <t xml:space="preserve">unknown </t>
+  </si>
+  <si>
+    <t xml:space="preserve">multiple </t>
+  </si>
+  <si>
+    <t>TOTAL no of GS tools</t>
+  </si>
+  <si>
+    <t>PHASE 6/7</t>
+  </si>
+  <si>
+    <t>9 (56.3%)</t>
+  </si>
+  <si>
+    <t>2 (12.5%)</t>
+  </si>
+  <si>
+    <t>1 (6.3%)</t>
+  </si>
+  <si>
+    <t>3 (18.8%)</t>
+  </si>
+  <si>
+    <t>16 (16.5%)</t>
+  </si>
+  <si>
+    <t>PHASE 5</t>
+  </si>
+  <si>
+    <t>8 (88.9%)</t>
+  </si>
+  <si>
+    <t>2 (22.2%)</t>
+  </si>
+  <si>
+    <t>3 (33.3%)</t>
+  </si>
+  <si>
+    <t>9 (9.3%)</t>
+  </si>
+  <si>
+    <t>PHASE 4</t>
+  </si>
+  <si>
+    <t>23 (71.9%)</t>
+  </si>
+  <si>
+    <t>2 (6.3%)</t>
+  </si>
+  <si>
+    <t>5 (15.6%)</t>
+  </si>
+  <si>
+    <t>1 (3.1%)</t>
+  </si>
+  <si>
+    <t>6 (18.8%)</t>
+  </si>
+  <si>
+    <t>32 (33%)</t>
+  </si>
+  <si>
+    <t>PHASE 3</t>
+  </si>
+  <si>
+    <t>10 (55.6%)</t>
+  </si>
+  <si>
+    <t>2 (11.1%)</t>
+  </si>
+  <si>
+    <t>1 (5.6%)</t>
+  </si>
+  <si>
+    <t>7 (39.9%)</t>
+  </si>
+  <si>
+    <t>18 (18.6%)</t>
+  </si>
+  <si>
+    <t>PHASE 2</t>
+  </si>
+  <si>
+    <t>5 (31.3%)</t>
+  </si>
+  <si>
+    <t>4 (25%)</t>
+  </si>
+  <si>
+    <t>7 (43.8%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16 (16.5%) </t>
+  </si>
+  <si>
+    <t>PHASE 1</t>
+  </si>
+  <si>
+    <t>3 (75%)</t>
+  </si>
+  <si>
+    <t>1 (25%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 (4.1%) </t>
+  </si>
+  <si>
+    <t>unknown</t>
+  </si>
+  <si>
+    <t>1 (50%)</t>
+  </si>
+  <si>
+    <t>2 (2.1%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOTAL </t>
+  </si>
+  <si>
+    <t>59 (60.8%)</t>
+  </si>
+  <si>
+    <t>4 (4.1%)</t>
+  </si>
+  <si>
+    <t>5 (5.2%)</t>
+  </si>
+  <si>
+    <t>1 (~1%)</t>
+  </si>
+  <si>
+    <t>24 (24.7%)</t>
+  </si>
+  <si>
+    <t>12 (12.4%)</t>
+  </si>
+  <si>
+    <t>97 (100%)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -926,6 +1086,24 @@
       <name val="Arial Narrow"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -941,7 +1119,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -967,6 +1145,82 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -987,7 +1241,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1042,6 +1296,33 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="17">
@@ -4466,7 +4747,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
@@ -4705,4 +4986,294 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="19"/>
+      <c r="B1" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="27"/>
+    </row>
+    <row r="2" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="20"/>
+      <c r="B2" s="21" t="s">
+        <v>279</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>280</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>281</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>282</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>283</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>284</v>
+      </c>
+      <c r="H2" s="21" t="s">
+        <v>285</v>
+      </c>
+      <c r="I2" s="22" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="23" t="s">
+        <v>287</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>288</v>
+      </c>
+      <c r="C3" s="21">
+        <v>0</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>289</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>289</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>290</v>
+      </c>
+      <c r="G3" s="21" t="s">
+        <v>291</v>
+      </c>
+      <c r="H3" s="21" t="s">
+        <v>290</v>
+      </c>
+      <c r="I3" s="21" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="24" t="s">
+        <v>293</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>294</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>295</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>295</v>
+      </c>
+      <c r="E4" s="21">
+        <v>0</v>
+      </c>
+      <c r="F4" s="21">
+        <v>0</v>
+      </c>
+      <c r="G4" s="21">
+        <v>0</v>
+      </c>
+      <c r="H4" s="21" t="s">
+        <v>296</v>
+      </c>
+      <c r="I4" s="21" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="24" t="s">
+        <v>298</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>299</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>300</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>301</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>302</v>
+      </c>
+      <c r="F5" s="21">
+        <v>0</v>
+      </c>
+      <c r="G5" s="21" t="s">
+        <v>303</v>
+      </c>
+      <c r="H5" s="21" t="s">
+        <v>301</v>
+      </c>
+      <c r="I5" s="21" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="24" t="s">
+        <v>305</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>306</v>
+      </c>
+      <c r="C6" s="21">
+        <v>0</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>307</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>308</v>
+      </c>
+      <c r="F6" s="21">
+        <v>0</v>
+      </c>
+      <c r="G6" s="21" t="s">
+        <v>309</v>
+      </c>
+      <c r="H6" s="21" t="s">
+        <v>307</v>
+      </c>
+      <c r="I6" s="21" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="24" t="s">
+        <v>311</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>312</v>
+      </c>
+      <c r="C7" s="21">
+        <v>0</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>313</v>
+      </c>
+      <c r="E7" s="21">
+        <v>0</v>
+      </c>
+      <c r="F7" s="21">
+        <v>0</v>
+      </c>
+      <c r="G7" s="21" t="s">
+        <v>314</v>
+      </c>
+      <c r="H7" s="21">
+        <v>0</v>
+      </c>
+      <c r="I7" s="21" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="24" t="s">
+        <v>316</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>317</v>
+      </c>
+      <c r="C8" s="21">
+        <v>0</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>318</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>318</v>
+      </c>
+      <c r="F8" s="21">
+        <v>0</v>
+      </c>
+      <c r="G8" s="21">
+        <v>0</v>
+      </c>
+      <c r="H8" s="21" t="s">
+        <v>318</v>
+      </c>
+      <c r="I8" s="21" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="24" t="s">
+        <v>320</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>321</v>
+      </c>
+      <c r="C9" s="21">
+        <v>0</v>
+      </c>
+      <c r="D9" s="21">
+        <v>0</v>
+      </c>
+      <c r="E9" s="21">
+        <v>0</v>
+      </c>
+      <c r="F9" s="21">
+        <v>0</v>
+      </c>
+      <c r="G9" s="21" t="s">
+        <v>321</v>
+      </c>
+      <c r="H9" s="21">
+        <v>0</v>
+      </c>
+      <c r="I9" s="21" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="24" t="s">
+        <v>323</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>324</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>325</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>292</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>326</v>
+      </c>
+      <c r="F10" s="21" t="s">
+        <v>327</v>
+      </c>
+      <c r="G10" s="21" t="s">
+        <v>328</v>
+      </c>
+      <c r="H10" s="21" t="s">
+        <v>329</v>
+      </c>
+      <c r="I10" s="21" t="s">
+        <v>330</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>